<commit_message>
- add column {TenKhachHang}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoKho/Teamplate_BaoCaoHangXuatKhoTheoDichVuDinhLuong.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoKho/Teamplate_BaoCaoHangXuatKhoTheoDichVuDinhLuong.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Tổng cộng:</t>
   </si>
@@ -92,6 +92,24 @@
   </si>
   <si>
     <t>Biển số xe</t>
+  </si>
+  <si>
+    <t>Mã khách hàng</t>
+  </si>
+  <si>
+    <t>Tên khách hàng</t>
+  </si>
+  <si>
+    <t>Giá bán</t>
+  </si>
+  <si>
+    <t>Thành tiền</t>
+  </si>
+  <si>
+    <t>% Sử dụng</t>
+  </si>
+  <si>
+    <t>NV thực hiện</t>
   </si>
 </sst>
 </file>
@@ -255,7 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -390,6 +408,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -701,11 +728,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA29"/>
+  <dimension ref="A1:AG29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,27 +740,29 @@
     <col min="1" max="1" width="28.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="4" customWidth="1"/>
     <col min="3" max="4" width="22.28515625" style="25" customWidth="1"/>
-    <col min="5" max="8" width="22.28515625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="4" customWidth="1"/>
-    <col min="11" max="12" width="23.5703125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="18" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.5703125" style="6" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="27" style="4" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="18" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" style="6" customWidth="1"/>
-    <col min="21" max="21" width="20.5703125" style="6" customWidth="1"/>
-    <col min="22" max="22" width="18" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.5703125" style="6" customWidth="1"/>
-    <col min="24" max="24" width="18" style="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.5703125" style="6" customWidth="1"/>
-    <col min="26" max="26" width="27" style="26" customWidth="1"/>
+    <col min="5" max="10" width="22.28515625" style="29" customWidth="1"/>
+    <col min="11" max="11" width="27.140625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="4" customWidth="1"/>
+    <col min="13" max="14" width="23.5703125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="18" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18" style="6" customWidth="1"/>
+    <col min="19" max="19" width="18" style="47" customWidth="1"/>
+    <col min="20" max="20" width="20.5703125" style="6" customWidth="1"/>
+    <col min="21" max="21" width="32.7109375" style="4" customWidth="1"/>
+    <col min="22" max="22" width="18.140625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="27" style="4" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="18" style="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18" style="6" customWidth="1"/>
+    <col min="27" max="27" width="20.5703125" style="6" customWidth="1"/>
+    <col min="28" max="28" width="18" style="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.5703125" style="6" customWidth="1"/>
+    <col min="30" max="30" width="18" style="6" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.5703125" style="6" customWidth="1"/>
+    <col min="32" max="32" width="27" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>9</v>
       </c>
@@ -757,14 +786,20 @@
       <c r="S1" s="41"/>
       <c r="T1" s="41"/>
       <c r="U1" s="41"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="2"/>
-    </row>
-    <row r="2" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="2"/>
+    </row>
+    <row r="2" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42"/>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
@@ -786,13 +821,19 @@
       <c r="S2" s="42"/>
       <c r="T2" s="42"/>
       <c r="U2" s="42"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="13"/>
-    </row>
-    <row r="3" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V2" s="42"/>
+      <c r="W2" s="42"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="42"/>
+      <c r="Z2" s="42"/>
+      <c r="AA2" s="42"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="13"/>
+    </row>
+    <row r="3" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="4"/>
       <c r="C3" s="25"/>
@@ -801,26 +842,32 @@
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="6"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="47"/>
       <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
       <c r="Y3" s="6"/>
-      <c r="Z3" s="26"/>
-    </row>
-    <row r="4" spans="1:27" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="26"/>
+    </row>
+    <row r="4" spans="1:33" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="44" t="s">
         <v>10</v>
       </c>
@@ -830,35 +877,41 @@
       <c r="E4" s="45"/>
       <c r="F4" s="45"/>
       <c r="G4" s="45"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="43" t="s">
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
       <c r="L4" s="43"/>
       <c r="M4" s="43"/>
       <c r="N4" s="43"/>
-      <c r="O4" s="33" t="s">
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="36" t="s">
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="34"/>
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="35"/>
+      <c r="AB4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="W4" s="37"/>
-      <c r="X4" s="32" t="s">
+      <c r="AC4" s="37"/>
+      <c r="AD4" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="32"/>
-    </row>
-    <row r="5" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE4" s="32"/>
+      <c r="AF4" s="32"/>
+    </row>
+    <row r="5" spans="1:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
@@ -875,70 +928,88 @@
         <v>25</v>
       </c>
       <c r="F5" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="I5" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="J5" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="K5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="L5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="M5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="N5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="O5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="P5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="S5" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="V5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="W5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="R5" s="20" t="s">
+      <c r="X5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="21" t="s">
+      <c r="Y5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="21" t="s">
+      <c r="Z5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="U5" s="21" t="s">
+      <c r="AA5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="V5" s="17" t="s">
+      <c r="AB5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="W5" s="17" t="s">
+      <c r="AC5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="X5" s="22" t="s">
+      <c r="AD5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="Y5" s="22" t="s">
+      <c r="AE5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="Z5" s="23" t="s">
+      <c r="AF5" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="24"/>
@@ -947,26 +1018,32 @@
       <c r="F6" s="31"/>
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="5"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="49"/>
       <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
       <c r="Y6" s="5"/>
-      <c r="Z6" s="27"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="27"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="24"/>
@@ -975,26 +1052,32 @@
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="5"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="49"/>
       <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
       <c r="Y7" s="5"/>
-      <c r="Z7" s="27"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="27"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="24"/>
@@ -1003,26 +1086,32 @@
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="27"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="27"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="24"/>
@@ -1031,26 +1120,32 @@
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="5"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="49"/>
       <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
       <c r="Y9" s="5"/>
-      <c r="Z9" s="27"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="27"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="24"/>
@@ -1059,26 +1154,32 @@
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="5"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="49"/>
       <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
       <c r="Y10" s="5"/>
-      <c r="Z10" s="27"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="27"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="24"/>
@@ -1087,26 +1188,32 @@
       <c r="F11" s="31"/>
       <c r="G11" s="31"/>
       <c r="H11" s="31"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="5"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="49"/>
       <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
       <c r="Y11" s="5"/>
-      <c r="Z11" s="27"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="27"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="24"/>
@@ -1115,26 +1222,32 @@
       <c r="F12" s="31"/>
       <c r="G12" s="31"/>
       <c r="H12" s="31"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="5"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="49"/>
       <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
       <c r="Y12" s="5"/>
-      <c r="Z12" s="27"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="27"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="24"/>
@@ -1143,26 +1256,32 @@
       <c r="F13" s="31"/>
       <c r="G13" s="31"/>
       <c r="H13" s="31"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="5"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="49"/>
       <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
       <c r="Y13" s="5"/>
-      <c r="Z13" s="27"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="27"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="24"/>
@@ -1171,26 +1290,32 @@
       <c r="F14" s="31"/>
       <c r="G14" s="31"/>
       <c r="H14" s="31"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="5"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="49"/>
       <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
       <c r="Y14" s="5"/>
-      <c r="Z14" s="27"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="27"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="24"/>
@@ -1199,26 +1324,32 @@
       <c r="F15" s="31"/>
       <c r="G15" s="31"/>
       <c r="H15" s="31"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="5"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="49"/>
       <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
       <c r="Y15" s="5"/>
-      <c r="Z15" s="27"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="5"/>
+      <c r="AF15" s="27"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="24"/>
@@ -1227,26 +1358,32 @@
       <c r="F16" s="31"/>
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="5"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="49"/>
       <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="5"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
       <c r="Y16" s="5"/>
-      <c r="Z16" s="27"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="27"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="24"/>
@@ -1255,26 +1392,32 @@
       <c r="F17" s="31"/>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="5"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="49"/>
       <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
       <c r="Y17" s="5"/>
-      <c r="Z17" s="27"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="27"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="24"/>
@@ -1283,26 +1426,32 @@
       <c r="F18" s="31"/>
       <c r="G18" s="31"/>
       <c r="H18" s="31"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="5"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="49"/>
       <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
       <c r="Y18" s="5"/>
-      <c r="Z18" s="27"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="27"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="24"/>
@@ -1311,26 +1460,32 @@
       <c r="F19" s="31"/>
       <c r="G19" s="31"/>
       <c r="H19" s="31"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="5"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="49"/>
       <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
       <c r="Y19" s="5"/>
-      <c r="Z19" s="27"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="27"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="24"/>
@@ -1339,26 +1494,32 @@
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
       <c r="H20" s="31"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="5"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="49"/>
       <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
-      <c r="V20" s="5"/>
-      <c r="W20" s="5"/>
-      <c r="X20" s="5"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
       <c r="Y20" s="5"/>
-      <c r="Z20" s="27"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="27"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="24"/>
@@ -1367,26 +1528,32 @@
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="5"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="49"/>
       <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
       <c r="Y21" s="5"/>
-      <c r="Z21" s="27"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="27"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="24"/>
@@ -1395,26 +1562,32 @@
       <c r="F22" s="31"/>
       <c r="G22" s="31"/>
       <c r="H22" s="31"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="5"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="49"/>
       <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-      <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
       <c r="Y22" s="5"/>
-      <c r="Z22" s="27"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="27"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="24"/>
@@ -1423,26 +1596,32 @@
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="5"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="49"/>
       <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
       <c r="Y23" s="5"/>
-      <c r="Z23" s="27"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="27"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="24"/>
@@ -1451,26 +1630,32 @@
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="5"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="49"/>
       <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
       <c r="Y24" s="5"/>
-      <c r="Z24" s="27"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="5"/>
+      <c r="AC24" s="5"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="5"/>
+      <c r="AF24" s="27"/>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="24"/>
@@ -1479,26 +1664,32 @@
       <c r="F25" s="31"/>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="5"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="49"/>
       <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
       <c r="Y25" s="5"/>
-      <c r="Z25" s="27"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
+      <c r="AF25" s="27"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="24"/>
@@ -1507,26 +1698,32 @@
       <c r="F26" s="31"/>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="5"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="49"/>
       <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
       <c r="Y26" s="5"/>
-      <c r="Z26" s="27"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="27"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="24"/>
@@ -1535,26 +1732,32 @@
       <c r="F27" s="31"/>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="5"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="49"/>
       <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
-      <c r="X27" s="5"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
       <c r="Y27" s="5"/>
-      <c r="Z27" s="27"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="27"/>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="24"/>
@@ -1563,26 +1766,32 @@
       <c r="F28" s="31"/>
       <c r="G28" s="31"/>
       <c r="H28" s="31"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="5"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="49"/>
       <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
-      <c r="V28" s="5"/>
-      <c r="W28" s="5"/>
-      <c r="X28" s="5"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
       <c r="Y28" s="5"/>
-      <c r="Z28" s="27"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="27"/>
+    </row>
+    <row r="29" spans="1:32" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="38" t="s">
         <v>0</v>
       </c>
@@ -1602,44 +1811,50 @@
       <c r="O29" s="39"/>
       <c r="P29" s="39"/>
       <c r="Q29" s="39"/>
-      <c r="R29" s="40"/>
-      <c r="S29" s="7">
-        <f>SUM(S$6:S28)</f>
-        <v>0</v>
-      </c>
-      <c r="T29" s="7">
-        <f>SUM(T$6:T28)</f>
-        <v>0</v>
-      </c>
-      <c r="U29" s="7"/>
-      <c r="V29" s="7">
-        <f>SUM(V$6:V28)</f>
-        <v>0</v>
-      </c>
-      <c r="W29" s="7">
-        <f>SUM(W$6:W28)</f>
-        <v>0</v>
-      </c>
-      <c r="X29" s="7">
-        <f>SUM(X$6:X28)</f>
-        <v>0</v>
-      </c>
+      <c r="R29" s="39"/>
+      <c r="S29" s="39"/>
+      <c r="T29" s="39"/>
+      <c r="U29" s="39"/>
+      <c r="V29" s="39"/>
+      <c r="W29" s="39"/>
+      <c r="X29" s="40"/>
       <c r="Y29" s="7">
         <f>SUM(Y$6:Y28)</f>
         <v>0</v>
       </c>
-      <c r="Z29" s="28"/>
+      <c r="Z29" s="7">
+        <f>SUM(Z$6:Z28)</f>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7">
+        <f>SUM(AB$6:AB28)</f>
+        <v>0</v>
+      </c>
+      <c r="AC29" s="7">
+        <f>SUM(AC$6:AC28)</f>
+        <v>0</v>
+      </c>
+      <c r="AD29" s="7">
+        <f>SUM(AD$6:AD28)</f>
+        <v>0</v>
+      </c>
+      <c r="AE29" s="7">
+        <f>SUM(AE$6:AE28)</f>
+        <v>0</v>
+      </c>
+      <c r="AF29" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="A29:R29"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:U2"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="A29:X29"/>
+    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="A2:AA2"/>
+    <mergeCell ref="K4:T4"/>
+    <mergeCell ref="A4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>